<commit_message>
updated code commit by saquib
</commit_message>
<xml_diff>
--- a/TestApp/src/main/java/com/qa/testdata/TestCoalData.xlsx
+++ b/TestApp/src/main/java/com/qa/testdata/TestCoalData.xlsx
@@ -16,12 +16,21 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="5">
   <si>
     <t>Quantity</t>
   </si>
   <si>
     <t>BidPrice</t>
+  </si>
+  <si>
+    <t>40</t>
+  </si>
+  <si>
+    <t>50</t>
+  </si>
+  <si>
+    <t>1000</t>
   </si>
 </sst>
 </file>
@@ -57,8 +66,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -356,7 +366,7 @@
   <dimension ref="A1:B3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+      <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -373,19 +383,19 @@
       </c>
     </row>
     <row r="2" spans="1:2">
-      <c r="A2">
-        <v>40</v>
-      </c>
-      <c r="B2">
-        <v>1000</v>
+      <c r="A2" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>4</v>
       </c>
     </row>
     <row r="3" spans="1:2">
-      <c r="A3">
-        <v>50</v>
-      </c>
-      <c r="B3">
-        <v>1000</v>
+      <c r="A3" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>4</v>
       </c>
     </row>
   </sheetData>

</xml_diff>